<commit_message>
prepare to run project
</commit_message>
<xml_diff>
--- a/Ремкомплекты.xlsx
+++ b/Ремкомплекты.xlsx
@@ -138,7 +138,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4762500" cy="4762500"/>
@@ -177,7 +177,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4762500" cy="4762500"/>
@@ -216,7 +216,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4762500" cy="4762500"/>
@@ -255,8 +255,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>17999</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4762500" cy="4762500"/>
     <xdr:pic>

</xml_diff>